<commit_message>
Continued progress on language exception handling. WIP.
</commit_message>
<xml_diff>
--- a/test/files/language-testing.xlsx
+++ b/test/files/language-testing.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7510" uniqueCount="2425">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7513" uniqueCount="2428">
   <si>
     <t>type</t>
   </si>
@@ -7940,6 +7940,15 @@
   </si>
   <si>
     <t>ppp_input::English</t>
+  </si>
+  <si>
+    <t>default_languageXXX</t>
+  </si>
+  <si>
+    <t>Huh?</t>
+  </si>
+  <si>
+    <t>label::Huh?</t>
   </si>
 </sst>
 </file>
@@ -8152,7 +8161,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1083">
+  <cellStyleXfs count="1085">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -9240,8 +9249,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -9446,8 +9457,14 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1083">
+  <cellStyles count="1085">
     <cellStyle name="20% - Accent6" xfId="816" builtinId="50"/>
     <cellStyle name="Excel Built-in Normal" xfId="228"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -9989,6 +10006,7 @@
     <cellStyle name="Followed Hyperlink" xfId="1078" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1080" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1082" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1084" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -10528,6 +10546,7 @@
     <cellStyle name="Hyperlink" xfId="1077" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1079" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1081" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1083" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="37"/>
     <cellStyle name="Normal 5" xfId="231"/>
@@ -10854,10 +10873,10 @@
   <dimension ref="A1:IX373"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="AR2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="BI2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="BA1" sqref="BA1"/>
+      <selection pane="bottomRight" activeCell="BJ2" sqref="BJ2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0"/>
@@ -10893,7 +10912,7 @@
     <col min="53" max="16384" width="8.6640625" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:61" ht="13" customHeight="1">
+    <row r="1" spans="1:62" ht="13" customHeight="1">
       <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
@@ -11071,8 +11090,11 @@
       <c r="BI1" s="40" t="s">
         <v>2423</v>
       </c>
-    </row>
-    <row r="2" spans="1:61" ht="13" customHeight="1">
+      <c r="BJ1" s="58" t="s">
+        <v>2427</v>
+      </c>
+    </row>
+    <row r="2" spans="1:62" ht="13" customHeight="1">
       <c r="A2" s="40" t="s">
         <v>14</v>
       </c>
@@ -11113,7 +11135,7 @@
       <c r="AZ2" s="67"/>
       <c r="BA2" s="67"/>
     </row>
-    <row r="3" spans="1:61" ht="13" customHeight="1">
+    <row r="3" spans="1:62" ht="13" customHeight="1">
       <c r="A3" s="40" t="s">
         <v>16</v>
       </c>
@@ -11156,7 +11178,7 @@
       <c r="AZ3" s="67"/>
       <c r="BA3" s="67"/>
     </row>
-    <row r="4" spans="1:61" ht="13" customHeight="1">
+    <row r="4" spans="1:62" ht="13" customHeight="1">
       <c r="A4" s="40" t="s">
         <v>20</v>
       </c>
@@ -11221,7 +11243,7 @@
       <c r="AZ4" s="67"/>
       <c r="BA4" s="67"/>
     </row>
-    <row r="5" spans="1:61" ht="13" customHeight="1">
+    <row r="5" spans="1:62" ht="13" customHeight="1">
       <c r="A5" s="40" t="s">
         <v>23</v>
       </c>
@@ -11288,7 +11310,7 @@
       <c r="AZ5" s="67"/>
       <c r="BA5" s="67"/>
     </row>
-    <row r="6" spans="1:61" ht="13" customHeight="1">
+    <row r="6" spans="1:62" ht="13" customHeight="1">
       <c r="A6" s="40" t="s">
         <v>27</v>
       </c>
@@ -11327,7 +11349,7 @@
       <c r="AZ6" s="67"/>
       <c r="BA6" s="67"/>
     </row>
-    <row r="7" spans="1:61" ht="13" customHeight="1">
+    <row r="7" spans="1:62" ht="13" customHeight="1">
       <c r="A7" s="40" t="s">
         <v>28</v>
       </c>
@@ -11396,7 +11418,7 @@
       <c r="AZ7" s="67"/>
       <c r="BA7" s="67"/>
     </row>
-    <row r="8" spans="1:61" ht="13" customHeight="1">
+    <row r="8" spans="1:62" ht="13" customHeight="1">
       <c r="A8" s="40" t="s">
         <v>32</v>
       </c>
@@ -11467,7 +11489,7 @@
       <c r="AZ8" s="67"/>
       <c r="BA8" s="67"/>
     </row>
-    <row r="9" spans="1:61" ht="13" customHeight="1">
+    <row r="9" spans="1:62" ht="13" customHeight="1">
       <c r="A9" s="40" t="s">
         <v>37</v>
       </c>
@@ -11538,7 +11560,7 @@
       <c r="AZ9" s="67"/>
       <c r="BA9" s="67"/>
     </row>
-    <row r="10" spans="1:61" ht="13" customHeight="1">
+    <row r="10" spans="1:62" ht="13" customHeight="1">
       <c r="A10" s="40" t="s">
         <v>16</v>
       </c>
@@ -11581,7 +11603,7 @@
       <c r="AZ10" s="31"/>
       <c r="BA10" s="31"/>
     </row>
-    <row r="11" spans="1:61" ht="13" customHeight="1">
+    <row r="11" spans="1:62" ht="13" customHeight="1">
       <c r="A11" s="40" t="s">
         <v>37</v>
       </c>
@@ -11649,7 +11671,7 @@
       <c r="AZ11" s="67"/>
       <c r="BA11" s="67"/>
     </row>
-    <row r="12" spans="1:61" ht="13" customHeight="1">
+    <row r="12" spans="1:62" ht="13" customHeight="1">
       <c r="A12" s="40" t="s">
         <v>37</v>
       </c>
@@ -11717,7 +11739,7 @@
       <c r="AZ12" s="67"/>
       <c r="BA12" s="67"/>
     </row>
-    <row r="13" spans="1:61" ht="13" customHeight="1">
+    <row r="13" spans="1:62" ht="13" customHeight="1">
       <c r="A13" s="40" t="s">
         <v>37</v>
       </c>
@@ -11785,7 +11807,7 @@
       <c r="AZ13" s="67"/>
       <c r="BA13" s="67"/>
     </row>
-    <row r="14" spans="1:61" ht="13" customHeight="1">
+    <row r="14" spans="1:62" ht="13" customHeight="1">
       <c r="A14" s="40" t="s">
         <v>37</v>
       </c>
@@ -11853,7 +11875,7 @@
       <c r="AZ14" s="67"/>
       <c r="BA14" s="67"/>
     </row>
-    <row r="15" spans="1:61" ht="13" customHeight="1">
+    <row r="15" spans="1:62" ht="13" customHeight="1">
       <c r="A15" s="40" t="s">
         <v>45</v>
       </c>
@@ -11922,7 +11944,7 @@
       <c r="AZ15" s="67"/>
       <c r="BA15" s="67"/>
     </row>
-    <row r="16" spans="1:61" ht="13" customHeight="1">
+    <row r="16" spans="1:62" ht="13" customHeight="1">
       <c r="A16" s="40" t="s">
         <v>45</v>
       </c>
@@ -35507,7 +35529,7 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0"/>
@@ -35533,8 +35555,8 @@
       <c r="D1" s="29" t="s">
         <v>1100</v>
       </c>
-      <c r="E1" s="13" t="s">
-        <v>1190</v>
+      <c r="E1" s="71" t="s">
+        <v>327</v>
       </c>
       <c r="F1" s="13" t="s">
         <v>1191</v>
@@ -45507,60 +45529,70 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="92.5" customWidth="1"/>
+    <col min="3" max="4" width="19.1640625" customWidth="1"/>
+    <col min="7" max="7" width="92.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" s="13" t="s">
         <v>597</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>598</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="71" t="s">
         <v>599</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="71" t="s">
+        <v>2425</v>
+      </c>
+      <c r="E1" s="13" t="s">
         <v>602</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="F1" s="13" t="s">
         <v>993</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>991</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="14" customFormat="1" ht="70">
+    <row r="2" spans="1:7" s="14" customFormat="1" ht="70">
       <c r="A2" s="39" t="s">
         <v>2282</v>
       </c>
       <c r="B2" s="18" t="s">
         <v>2283</v>
       </c>
-      <c r="C2" s="18" t="s">
-        <v>1084</v>
-      </c>
-      <c r="D2" s="18" t="b">
+      <c r="C2" s="72" t="s">
+        <v>2426</v>
+      </c>
+      <c r="D2" s="72" t="s">
+        <v>2426</v>
+      </c>
+      <c r="E2" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="F2" s="18" t="s">
         <v>994</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="G2" s="12" t="s">
         <v>992</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Added some language error checks. Added error logging to stderr.
</commit_message>
<xml_diff>
--- a/test/files/language-testing.xlsx
+++ b/test/files/language-testing.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="27526"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="26500" tabRatio="443"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="26500" tabRatio="443" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -10872,11 +10872,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IX373"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="BI2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="BJ2" sqref="BJ2"/>
+      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0"/>
@@ -45531,9 +45531,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>

</xml_diff>